<commit_message>
feat : date-wise plotting
</commit_message>
<xml_diff>
--- a/data/gcs_data.xlsx
+++ b/data/gcs_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\Projects\DataVisualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\Projects\DataVisualization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E3CE04-EAB2-4503-ACED-088C3565D5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D5786-74BC-419A-9836-FF5B3404892D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,10 +43,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,10 +79,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>0.17708333333333334</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="D6">
         <v>1220</v>
@@ -529,10 +537,108 @@
         <v>2</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="D12">
         <v>1250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="D13">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D14">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D15">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D16">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D17">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>45077</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="D18">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>45077</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D19">
+        <v>1116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>